<commit_message>
create_glycontact_annotated_graph, works except for 3FUC
</commit_message>
<xml_diff>
--- a/scripts/correlation/metric_df/AAL_metrics.xlsx
+++ b/scripts/correlation/metric_df/AAL_metrics.xlsx
@@ -545,7 +545,11 @@
       <c r="F4" t="n">
         <v>9.644567140000001</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -568,7 +572,11 @@
       <c r="F5" t="n">
         <v>3.889493000000007</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -618,7 +626,11 @@
       <c r="F7" t="n">
         <v>11.43067193333333</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -641,7 +653,11 @@
       <c r="F8" t="n">
         <v>8.653719799999996</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -691,7 +707,11 @@
       <c r="F10" t="n">
         <v>2.578956608160815</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -714,7 +734,11 @@
       <c r="F11" t="n">
         <v>8.504671733840048</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -791,7 +815,11 @@
       <c r="F14" t="n">
         <v>18.36697768223178</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -841,7 +869,11 @@
       <c r="F16" t="n">
         <v>2.219634240000001</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -864,7 +896,11 @@
       <c r="F17" t="n">
         <v>6.404429833333334</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -968,7 +1004,11 @@
       <c r="F21" t="n">
         <v>4.275120000000004</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1099,7 +1139,11 @@
       <c r="F26" t="n">
         <v>17.92982791136256</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1122,7 +1166,11 @@
       <c r="F27" t="n">
         <v>11.90423596</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1226,7 +1274,11 @@
       <c r="F31" t="n">
         <v>6.011923522352238</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>lipid/free</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">

</xml_diff>